<commit_message>
Rename GCost parameter startup, shutdown as csu, csd
</commit_message>
<xml_diff>
--- a/ams/cases/ieee14/ieee14.xlsx
+++ b/ams/cases/ieee14/ieee14.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/ams/ams/cases/ieee14/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3EF610-C141-4643-8CC9-651790A5C31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36480" yWindow="1540" windowWidth="35300" windowHeight="19000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28800" windowHeight="12540" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -22,7 +16,7 @@
     <sheet name="Area" sheetId="7" r:id="rId7"/>
     <sheet name="GCost" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -494,6 +488,9 @@
     <t>phi</t>
   </si>
   <si>
+    <t>rate_a</t>
+  </si>
+  <si>
     <t>Line_1</t>
   </si>
   <si>
@@ -719,10 +716,10 @@
     <t>type</t>
   </si>
   <si>
-    <t>startup</t>
-  </si>
-  <si>
-    <t>shutdown</t>
+    <t>csu</t>
+  </si>
+  <si>
+    <t>csd</t>
   </si>
   <si>
     <t>c2</t>
@@ -759,33 +756,373 @@
   </si>
   <si>
     <t>GCOST_5</t>
-  </si>
-  <si>
-    <t>rate_a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -793,24 +1130,310 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1132,21 +1755,21 @@
       </a:style>
     </a:lnDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1190,7 +1813,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1234,7 +1857,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1278,7 +1901,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1322,7 +1945,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1366,7 +1989,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1410,7 +2033,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1454,7 +2077,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -1498,7 +2121,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -1542,7 +2165,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -1586,7 +2209,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -1630,7 +2253,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -1674,7 +2297,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -1718,7 +2341,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -1762,7 +2385,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -1808,6 +2431,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
   <ignoredErrors>
     <ignoredError sqref="A1:N15" numberStoredAsText="1"/>
   </ignoredErrors>
@@ -1815,14 +2439,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="4"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1881,7 +2508,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1937,7 +2564,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1993,7 +2620,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2049,7 +2676,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -2107,6 +2734,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
   <ignoredErrors>
     <ignoredError sqref="A1:S5" numberStoredAsText="1"/>
   </ignoredErrors>
@@ -2114,14 +2742,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="1"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2183,7 +2814,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2244,6 +2875,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
   <ignoredErrors>
     <ignoredError sqref="A1:T2" numberStoredAsText="1"/>
   </ignoredErrors>
@@ -2251,14 +2883,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2293,7 +2928,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2328,7 +2963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2363,7 +2998,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2398,7 +3033,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -2433,7 +3068,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -2468,7 +3103,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -2503,7 +3138,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -2538,7 +3173,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -2573,7 +3208,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -2608,7 +3243,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -2643,7 +3278,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -2680,6 +3315,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
   <ignoredErrors>
     <ignoredError sqref="A1:K12" numberStoredAsText="1"/>
   </ignoredErrors>
@@ -2687,16 +3323,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:Y21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" topLeftCell="I1" workbookViewId="0">
       <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2770,21 +3407,21 @@
         <v>10</v>
       </c>
       <c r="Y1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
@@ -2796,7 +3433,7 @@
         <v>86</v>
       </c>
       <c r="H2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I2" t="s">
         <v>17</v>
@@ -2805,13 +3442,13 @@
         <v>17</v>
       </c>
       <c r="K2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="L2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="N2" t="s">
         <v>14</v>
@@ -2841,18 +3478,18 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
@@ -2864,7 +3501,7 @@
         <v>86</v>
       </c>
       <c r="H3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I3" t="s">
         <v>17</v>
@@ -2873,13 +3510,13 @@
         <v>17</v>
       </c>
       <c r="K3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="L3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="M3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N3" t="s">
         <v>14</v>
@@ -2909,18 +3546,18 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E4" t="s">
         <v>21</v>
@@ -2932,7 +3569,7 @@
         <v>86</v>
       </c>
       <c r="H4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I4" t="s">
         <v>17</v>
@@ -2941,13 +3578,13 @@
         <v>17</v>
       </c>
       <c r="K4" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="L4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="M4" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="N4" t="s">
         <v>14</v>
@@ -2977,18 +3614,18 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E5" t="s">
         <v>21</v>
@@ -3000,7 +3637,7 @@
         <v>86</v>
       </c>
       <c r="H5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I5" t="s">
         <v>17</v>
@@ -3009,13 +3646,13 @@
         <v>17</v>
       </c>
       <c r="K5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="M5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="N5" t="s">
         <v>14</v>
@@ -3045,18 +3682,18 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
@@ -3068,7 +3705,7 @@
         <v>86</v>
       </c>
       <c r="H6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I6" t="s">
         <v>17</v>
@@ -3077,13 +3714,13 @@
         <v>17</v>
       </c>
       <c r="K6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="L6" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="M6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="N6" t="s">
         <v>14</v>
@@ -3113,18 +3750,18 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E7" t="s">
         <v>25</v>
@@ -3136,7 +3773,7 @@
         <v>86</v>
       </c>
       <c r="H7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I7" t="s">
         <v>17</v>
@@ -3145,13 +3782,13 @@
         <v>17</v>
       </c>
       <c r="K7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="L7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="M7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="N7" t="s">
         <v>14</v>
@@ -3181,18 +3818,18 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E8" t="s">
         <v>29</v>
@@ -3204,7 +3841,7 @@
         <v>86</v>
       </c>
       <c r="H8" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I8" t="s">
         <v>17</v>
@@ -3213,10 +3850,10 @@
         <v>17</v>
       </c>
       <c r="K8" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="L8" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="M8" t="s">
         <v>14</v>
@@ -3249,18 +3886,18 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25">
       <c r="A9" t="s">
         <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E9" t="s">
         <v>37</v>
@@ -3272,7 +3909,7 @@
         <v>86</v>
       </c>
       <c r="H9" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I9" t="s">
         <v>39</v>
@@ -3281,10 +3918,10 @@
         <v>39</v>
       </c>
       <c r="K9" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="L9" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="M9" t="s">
         <v>14</v>
@@ -3317,18 +3954,18 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25">
       <c r="A10" t="s">
         <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E10" t="s">
         <v>37</v>
@@ -3340,7 +3977,7 @@
         <v>86</v>
       </c>
       <c r="H10" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I10" t="s">
         <v>39</v>
@@ -3349,10 +3986,10 @@
         <v>39</v>
       </c>
       <c r="K10" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="L10" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="M10" t="s">
         <v>14</v>
@@ -3385,18 +4022,18 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25">
       <c r="A11" t="s">
         <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E11" t="s">
         <v>37</v>
@@ -3408,7 +4045,7 @@
         <v>86</v>
       </c>
       <c r="H11" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I11" t="s">
         <v>39</v>
@@ -3417,10 +4054,10 @@
         <v>39</v>
       </c>
       <c r="K11" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="L11" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="M11" t="s">
         <v>14</v>
@@ -3453,18 +4090,18 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25">
       <c r="A12" t="s">
         <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C12" t="s">
         <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E12" t="s">
         <v>42</v>
@@ -3476,7 +4113,7 @@
         <v>86</v>
       </c>
       <c r="H12" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I12" t="s">
         <v>39</v>
@@ -3488,7 +4125,7 @@
         <v>14</v>
       </c>
       <c r="L12" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="M12" t="s">
         <v>14</v>
@@ -3521,18 +4158,18 @@
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25">
       <c r="A13" t="s">
         <v>58</v>
       </c>
       <c r="B13" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C13" t="s">
         <v>15</v>
       </c>
       <c r="D13" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E13" t="s">
         <v>50</v>
@@ -3544,7 +4181,7 @@
         <v>86</v>
       </c>
       <c r="H13" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I13" t="s">
         <v>39</v>
@@ -3553,10 +4190,10 @@
         <v>39</v>
       </c>
       <c r="K13" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="L13" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="M13" t="s">
         <v>14</v>
@@ -3589,18 +4226,18 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25">
       <c r="A14" t="s">
         <v>62</v>
       </c>
       <c r="B14" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C14" t="s">
         <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E14" t="s">
         <v>50</v>
@@ -3612,7 +4249,7 @@
         <v>86</v>
       </c>
       <c r="H14" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I14" t="s">
         <v>39</v>
@@ -3621,10 +4258,10 @@
         <v>39</v>
       </c>
       <c r="K14" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="L14" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="M14" t="s">
         <v>14</v>
@@ -3657,18 +4294,18 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25">
       <c r="A15" t="s">
         <v>66</v>
       </c>
       <c r="B15" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C15" t="s">
         <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E15" t="s">
         <v>54</v>
@@ -3680,7 +4317,7 @@
         <v>86</v>
       </c>
       <c r="H15" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I15" t="s">
         <v>39</v>
@@ -3689,10 +4326,10 @@
         <v>39</v>
       </c>
       <c r="K15" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="L15" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="M15" t="s">
         <v>14</v>
@@ -3725,18 +4362,18 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25">
       <c r="A16" t="s">
         <v>70</v>
       </c>
       <c r="B16" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E16" t="s">
         <v>62</v>
@@ -3748,7 +4385,7 @@
         <v>86</v>
       </c>
       <c r="H16" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I16" t="s">
         <v>39</v>
@@ -3757,10 +4394,10 @@
         <v>39</v>
       </c>
       <c r="K16" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="L16" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="M16" t="s">
         <v>14</v>
@@ -3793,18 +4430,18 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25">
       <c r="A17" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B17" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C17" t="s">
         <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E17" t="s">
         <v>66</v>
@@ -3816,7 +4453,7 @@
         <v>86</v>
       </c>
       <c r="H17" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I17" t="s">
         <v>39</v>
@@ -3825,10 +4462,10 @@
         <v>39</v>
       </c>
       <c r="K17" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="L17" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M17" t="s">
         <v>14</v>
@@ -3861,18 +4498,18 @@
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25">
       <c r="A18" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B18" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C18" t="s">
         <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E18" t="s">
         <v>29</v>
@@ -3884,7 +4521,7 @@
         <v>86</v>
       </c>
       <c r="H18" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I18" t="s">
         <v>17</v>
@@ -3896,7 +4533,7 @@
         <v>14</v>
       </c>
       <c r="L18" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="M18" t="s">
         <v>14</v>
@@ -3920,7 +4557,7 @@
         <v>15</v>
       </c>
       <c r="T18" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="U18" t="s">
         <v>14</v>
@@ -3929,18 +4566,18 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25">
       <c r="A19" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B19" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C19" t="s">
         <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E19" t="s">
         <v>29</v>
@@ -3952,7 +4589,7 @@
         <v>86</v>
       </c>
       <c r="H19" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I19" t="s">
         <v>17</v>
@@ -3964,7 +4601,7 @@
         <v>14</v>
       </c>
       <c r="L19" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="M19" t="s">
         <v>14</v>
@@ -3988,7 +4625,7 @@
         <v>15</v>
       </c>
       <c r="T19" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="U19" t="s">
         <v>14</v>
@@ -3997,18 +4634,18 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25">
       <c r="A20" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B20" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C20" t="s">
         <v>15</v>
       </c>
       <c r="D20" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E20" t="s">
         <v>37</v>
@@ -4020,7 +4657,7 @@
         <v>86</v>
       </c>
       <c r="H20" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I20" t="s">
         <v>39</v>
@@ -4032,7 +4669,7 @@
         <v>14</v>
       </c>
       <c r="L20" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="M20" t="s">
         <v>14</v>
@@ -4056,7 +4693,7 @@
         <v>15</v>
       </c>
       <c r="T20" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="U20" t="s">
         <v>14</v>
@@ -4065,18 +4702,18 @@
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25">
       <c r="A21" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B21" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C21" t="s">
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E21" t="s">
         <v>46</v>
@@ -4088,7 +4725,7 @@
         <v>86</v>
       </c>
       <c r="H21" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I21" t="s">
         <v>17</v>
@@ -4100,7 +4737,7 @@
         <v>14</v>
       </c>
       <c r="L21" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="M21" t="s">
         <v>14</v>
@@ -4124,7 +4761,7 @@
         <v>15</v>
       </c>
       <c r="T21" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="U21" t="s">
         <v>14</v>
@@ -4135,6 +4772,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
   <ignoredErrors>
     <ignoredError sqref="A1:X21" numberStoredAsText="1"/>
   </ignoredErrors>
@@ -4142,14 +4780,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4181,18 +4822,18 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E2" t="s">
         <v>50</v>
@@ -4207,24 +4848,24 @@
         <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="J2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E3" t="s">
         <v>70</v>
@@ -4242,11 +4883,12 @@
         <v>88</v>
       </c>
       <c r="J3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
   <ignoredErrors>
     <ignoredError sqref="A1:J3" numberStoredAsText="1"/>
   </ignoredErrors>
@@ -4254,14 +4896,17 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="2" outlineLevelCol="3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4275,7 +4920,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -4286,10 +4931,10 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -4300,11 +4945,12 @@
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
   <ignoredErrors>
     <ignoredError sqref="A1:D3" numberStoredAsText="1"/>
   </ignoredErrors>
@@ -4312,14 +4958,17 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="5"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4327,33 +4976,33 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="H1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="I1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C2" t="s">
         <v>104</v>
@@ -4368,21 +5017,21 @@
         <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="H2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C3" t="s">
         <v>85</v>
@@ -4400,18 +5049,18 @@
         <v>115</v>
       </c>
       <c r="H3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C4" t="s">
         <v>95</v>
@@ -4426,21 +5075,21 @@
         <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="H4" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="I4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C5" t="s">
         <v>98</v>
@@ -4455,21 +5104,21 @@
         <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="H5" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="I5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C6" t="s">
         <v>102</v>
@@ -4484,10 +5133,10 @@
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="H6" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="I6" t="s">
         <v>14</v>
@@ -4495,8 +5144,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="A1:I6" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:D1 G1:I1 A2:I6" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>